<commit_message>
16th of October #RECAP
</commit_message>
<xml_diff>
--- a/common/!Темы.xlsx
+++ b/common/!Темы.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="107">
   <si>
     <t>Название темы</t>
   </si>
@@ -329,13 +329,19 @@
   </si>
   <si>
     <t>Дебаггер</t>
+  </si>
+  <si>
+    <t>Иерархию исключений сделать отдельно</t>
+  </si>
+  <si>
+    <t>Инкапсуляция покрыта</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,8 +375,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,8 +402,18 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -391,20 +421,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,58 +809,58 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -982,19 +1036,19 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="7">
         <v>5</v>
       </c>
-      <c r="C19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1030,16 +1084,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1131,17 +1185,20 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>99</v>
+      <c r="C29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1159,16 +1216,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1423,16 +1480,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1510,16 +1567,16 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="4">
         <v>7</v>
       </c>
-      <c r="C55" t="s">
-        <v>87</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1564,6 +1621,9 @@
       <c r="D58" t="s">
         <v>99</v>
       </c>
+      <c r="E58" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1737,30 +1797,30 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71" t="s">
-        <v>86</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="B71" s="4">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C75" t="s">
-        <v>87</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="C75" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" s="7" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1807,30 +1867,30 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C79" t="s">
-        <v>87</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="C79" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C80" t="s">
-        <v>87</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="C80" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="7" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>